<commit_message>
update manual reference file
</commit_message>
<xml_diff>
--- a/inst/test_materials/codebook_manually_extracted_stats.xlsx
+++ b/inst/test_materials/codebook_manually_extracted_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnuijten\Documents\statcheck\inst\test_materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C4141C-2EB9-49AD-85EE-04925F3019DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62187719-B9D2-4DC5-80A9-D2B12EFE4DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{929BE018-39EC-4CD3-A4A1-C99C7C36096B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
   <si>
     <t>file_id</t>
   </si>
@@ -177,6 +177,45 @@
   </si>
   <si>
     <t>This is the codebook for the file "manually_extrected_stats.xlsx", used in the R package statcheck. This file contains manually extracted statistics from a non-random selection of published articles. It can be used to test if statcheck accurately extracts statistics from different file types and different reporting styles. It contains nicely formatted apa results, non-apa results, results with pdf conversion issues, and results with type-setting issues (e.g., spanning two pages).</t>
+  </si>
+  <si>
+    <t>typesetting_issues</t>
+  </si>
+  <si>
+    <t>are there typesetting issues? (e.g., result spanned two pages)</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>decision_error</t>
+  </si>
+  <si>
+    <t>one_tailed</t>
+  </si>
+  <si>
+    <t>p-value does not match degrees of freedom and test statistic</t>
+  </si>
+  <si>
+    <t>recomputed p-value is significant and reported is not, or vice versa</t>
+  </si>
+  <si>
+    <t>is this test explicitly identified as a one-tailed test in the text?</t>
+  </si>
+  <si>
+    <t>error_1tail</t>
+  </si>
+  <si>
+    <t>decision_error_1tail</t>
+  </si>
+  <si>
+    <t>is the result a decision error when taking into account one-tailed testing?</t>
+  </si>
+  <si>
+    <t>is the result an error when taking into account one-tailed testing?</t>
+  </si>
+  <si>
+    <t>logical</t>
   </si>
 </sst>
 </file>
@@ -306,13 +345,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -323,19 +361,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83EE38A7-6956-4E16-8DA5-0EB57A78F6DD}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,31 +702,31 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="19"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="15"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="15"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="14"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="15"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="14"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="17"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -706,8 +744,7 @@
       <c r="A13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -715,8 +752,7 @@
       <c r="A14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -724,10 +760,10 @@
       <c r="A15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -735,10 +771,10 @@
       <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -746,10 +782,10 @@
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -757,10 +793,10 @@
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -768,10 +804,10 @@
       <c r="A19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -779,10 +815,10 @@
       <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -790,10 +826,10 @@
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -801,10 +837,10 @@
       <c r="A22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -812,10 +848,10 @@
       <c r="A23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -823,10 +859,10 @@
       <c r="A24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -834,10 +870,10 @@
       <c r="A25" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -845,10 +881,10 @@
       <c r="A26" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -856,10 +892,10 @@
       <c r="A27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -867,10 +903,10 @@
       <c r="A28" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -878,10 +914,10 @@
       <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -889,43 +925,109 @@
       <c r="A30" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>40</v>
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B37" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
+      <c r="C37" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B39" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C39" s="8" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>